<commit_message>
Fix: Added the TestData
</commit_message>
<xml_diff>
--- a/src/test/resources/data/InsuranceData.xlsx
+++ b/src/test/resources/data/InsuranceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aarthy\friday-selenium-master\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366232A0-6F69-41D4-AF0F-69B4A64565C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2540C7-3086-4355-BC32-88C5290D9942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{9D1CEB55-4E9A-4C87-A8C6-4245FC135435}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Testcase name</t>
   </si>
@@ -57,7 +57,19 @@
     <t>Cabrio</t>
   </si>
   <si>
-    <t>BMW Add car</t>
+    <t>null</t>
+  </si>
+  <si>
+    <t>BMW 1er Model</t>
+  </si>
+  <si>
+    <t>Insurancestatus</t>
+  </si>
+  <si>
+    <t>Modify</t>
+  </si>
+  <si>
+    <t>carhsn</t>
   </si>
 </sst>
 </file>
@@ -410,43 +422,57 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAE2075-1E66-4BC7-AA40-8D66F31DB9A3}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the TestData with the testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/data/InsuranceData.xlsx
+++ b/src/test/resources/data/InsuranceData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aarthy\friday-selenium-master\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaselvaraj\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2540C7-3086-4355-BC32-88C5290D9942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C64342D-865E-4B77-A641-F7CE14807F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{9D1CEB55-4E9A-4C87-A8C6-4245FC135435}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="19200" windowHeight="10200" xr2:uid="{9D1CEB55-4E9A-4C87-A8C6-4245FC135435}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>Testcase name</t>
   </si>
@@ -57,19 +57,94 @@
     <t>Cabrio</t>
   </si>
   <si>
+    <t>X1</t>
+  </si>
+  <si>
     <t>null</t>
   </si>
   <si>
+    <t>AUDI</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Kombi</t>
+  </si>
+  <si>
+    <t>FORD</t>
+  </si>
+  <si>
+    <t>Fiesta</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>Kuga</t>
+  </si>
+  <si>
+    <t>Geschlossen</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
     <t>BMW 1er Model</t>
   </si>
   <si>
+    <t>BMW X1 Model</t>
+  </si>
+  <si>
+    <t>BMW X3 Model</t>
+  </si>
+  <si>
+    <t>AUDI A1  Model</t>
+  </si>
+  <si>
+    <t>AUDI A4  Model</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>AUDI A5  Model</t>
+  </si>
+  <si>
+    <t>FORD Fiesta  Model</t>
+  </si>
+  <si>
+    <t>FORD Focus  Model</t>
+  </si>
+  <si>
+    <t>FORD Kuga  Model</t>
+  </si>
+  <si>
     <t>Insurancestatus</t>
   </si>
   <si>
+    <t>Purchase</t>
+  </si>
+  <si>
     <t>Modify</t>
   </si>
   <si>
     <t>carhsn</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz</t>
+  </si>
+  <si>
+    <t>A class</t>
+  </si>
+  <si>
+    <t>Benz A class Model</t>
+  </si>
+  <si>
+    <t>10.2020:0708:472</t>
   </si>
 </sst>
 </file>
@@ -422,17 +497,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAE2075-1E66-4BC7-AA40-8D66F31DB9A3}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -440,7 +515,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -452,15 +527,15 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -472,7 +547,187 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>